<commit_message>
debug code for missing last dash; fixed GPS DO
</commit_message>
<xml_diff>
--- a/Docs/misc/wall_ticks_mod.xlsx
+++ b/Docs/misc/wall_ticks_mod.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23913"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="940" yWindow="620" windowWidth="25940" windowHeight="21720" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
   <si>
     <t>Hour</t>
   </si>
@@ -131,8 +132,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="33">
+  <cellStyleXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -175,7 +178,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="33">
+  <cellStyles count="35">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -192,6 +195,7 @@
     <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -208,6 +212,7 @@
     <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2052,7 +2057,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q208"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N25" sqref="N25"/>
     </sheetView>
   </sheetViews>
@@ -2168,7 +2173,7 @@
         <v>10</v>
       </c>
       <c r="P3">
-        <f t="shared" ref="P3:P21" si="1">(N3*60)+O3</f>
+        <f t="shared" ref="P3:P6" si="1">(N3*60)+O3</f>
         <v>10</v>
       </c>
       <c r="Q3">
@@ -4705,6 +4710,152 @@
       <c r="L208">
         <f t="shared" si="12"/>
         <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1">
+        <v>0</v>
+      </c>
+      <c r="C1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="B2">
+        <f>B1+3</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="B3">
+        <f t="shared" ref="B3:B21" si="0">B2+3</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="B4">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="B5">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="B6">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="B7">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="B8">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="B9">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="B10">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="B11">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="B12">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="B13">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="B14">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="B15">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="B16">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2">
+      <c r="B17">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2">
+      <c r="B18">
+        <f t="shared" si="0"/>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2">
+      <c r="B19">
+        <f t="shared" si="0"/>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2">
+      <c r="B20">
+        <f t="shared" si="0"/>
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
clean up LCD display. fix rig setup regression.  LCD changes cause delay new vlaue ot be 468
</commit_message>
<xml_diff>
--- a/Docs/misc/wall_ticks_mod.xlsx
+++ b/Docs/misc/wall_ticks_mod.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23913"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
   <si>
     <t>Hour</t>
   </si>
@@ -69,6 +70,15 @@
   </si>
   <si>
     <t>strick</t>
+  </si>
+  <si>
+    <t>Wall Tick</t>
+  </si>
+  <si>
+    <t>slot start time</t>
+  </si>
+  <si>
+    <t>sked tick</t>
   </si>
 </sst>
 </file>
@@ -132,8 +142,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="35">
+  <cellStyleXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -178,7 +194,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="35">
+  <cellStyles count="41">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -196,6 +212,9 @@
     <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -213,6 +232,9 @@
     <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -544,7 +566,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E123"/>
   <sheetViews>
-    <sheetView topLeftCell="A41" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D62" sqref="D62"/>
     </sheetView>
   </sheetViews>
@@ -2057,7 +2079,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q208"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="N25" sqref="N25"/>
     </sheetView>
   </sheetViews>
@@ -4727,7 +4749,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
@@ -4752,7 +4774,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="B3">
-        <f t="shared" ref="B3:B21" si="0">B2+3</f>
+        <f t="shared" ref="B3:B20" si="0">B2+3</f>
         <v>6</v>
       </c>
     </row>
@@ -4856,6 +4878,2383 @@
       <c r="B20">
         <f t="shared" si="0"/>
         <v>57</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F182"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <f>A3-$F$1</f>
+        <v>-30</v>
+      </c>
+      <c r="C3">
+        <f t="shared" ref="C3:C21" si="0">180-ABS(B3)</f>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <f t="shared" ref="B4:B67" si="1">A4-$F$1</f>
+        <v>-29</v>
+      </c>
+      <c r="C4">
+        <f t="shared" si="0"/>
+        <v>151</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <f t="shared" si="1"/>
+        <v>-28</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>152</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6">
+        <f t="shared" si="1"/>
+        <v>-27</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>153</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7">
+        <v>4</v>
+      </c>
+      <c r="B7">
+        <f t="shared" si="1"/>
+        <v>-26</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>154</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8">
+        <v>5</v>
+      </c>
+      <c r="B8">
+        <f t="shared" si="1"/>
+        <v>-25</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>155</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9">
+        <v>6</v>
+      </c>
+      <c r="B9">
+        <f t="shared" si="1"/>
+        <v>-24</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>156</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10">
+        <v>7</v>
+      </c>
+      <c r="B10">
+        <f t="shared" si="1"/>
+        <v>-23</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>157</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11">
+        <v>8</v>
+      </c>
+      <c r="B11">
+        <f t="shared" si="1"/>
+        <v>-22</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>158</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12">
+        <v>9</v>
+      </c>
+      <c r="B12">
+        <f t="shared" si="1"/>
+        <v>-21</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>159</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13">
+        <v>10</v>
+      </c>
+      <c r="B13">
+        <f t="shared" si="1"/>
+        <v>-20</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="0"/>
+        <v>160</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14">
+        <v>11</v>
+      </c>
+      <c r="B14">
+        <f t="shared" si="1"/>
+        <v>-19</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="0"/>
+        <v>161</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15">
+        <v>12</v>
+      </c>
+      <c r="B15">
+        <f t="shared" si="1"/>
+        <v>-18</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="0"/>
+        <v>162</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16">
+        <v>13</v>
+      </c>
+      <c r="B16">
+        <f t="shared" si="1"/>
+        <v>-17</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="0"/>
+        <v>163</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17">
+        <v>14</v>
+      </c>
+      <c r="B17">
+        <f t="shared" si="1"/>
+        <v>-16</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="0"/>
+        <v>164</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18">
+        <v>15</v>
+      </c>
+      <c r="B18">
+        <f t="shared" si="1"/>
+        <v>-15</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="0"/>
+        <v>165</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19">
+        <v>16</v>
+      </c>
+      <c r="B19">
+        <f t="shared" si="1"/>
+        <v>-14</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="0"/>
+        <v>166</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20">
+        <v>17</v>
+      </c>
+      <c r="B20">
+        <f t="shared" si="1"/>
+        <v>-13</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="0"/>
+        <v>167</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21">
+        <v>18</v>
+      </c>
+      <c r="B21">
+        <f t="shared" si="1"/>
+        <v>-12</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="0"/>
+        <v>168</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22">
+        <v>19</v>
+      </c>
+      <c r="B22">
+        <f t="shared" si="1"/>
+        <v>-11</v>
+      </c>
+      <c r="C22">
+        <f>180-ABS(B22)</f>
+        <v>169</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23">
+        <v>20</v>
+      </c>
+      <c r="B23">
+        <f t="shared" si="1"/>
+        <v>-10</v>
+      </c>
+      <c r="C23">
+        <f t="shared" ref="C23:C86" si="2">180-ABS(B23)</f>
+        <v>170</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24">
+        <v>21</v>
+      </c>
+      <c r="B24">
+        <f t="shared" si="1"/>
+        <v>-9</v>
+      </c>
+      <c r="C24">
+        <f t="shared" si="2"/>
+        <v>171</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25">
+        <v>22</v>
+      </c>
+      <c r="B25">
+        <f t="shared" si="1"/>
+        <v>-8</v>
+      </c>
+      <c r="C25">
+        <f t="shared" si="2"/>
+        <v>172</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26">
+        <v>23</v>
+      </c>
+      <c r="B26">
+        <f t="shared" si="1"/>
+        <v>-7</v>
+      </c>
+      <c r="C26">
+        <f t="shared" si="2"/>
+        <v>173</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27">
+        <v>24</v>
+      </c>
+      <c r="B27">
+        <f t="shared" si="1"/>
+        <v>-6</v>
+      </c>
+      <c r="C27">
+        <f t="shared" si="2"/>
+        <v>174</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28">
+        <v>25</v>
+      </c>
+      <c r="B28">
+        <f t="shared" si="1"/>
+        <v>-5</v>
+      </c>
+      <c r="C28">
+        <f t="shared" si="2"/>
+        <v>175</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29">
+        <v>26</v>
+      </c>
+      <c r="B29">
+        <f t="shared" si="1"/>
+        <v>-4</v>
+      </c>
+      <c r="C29">
+        <f t="shared" si="2"/>
+        <v>176</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30">
+        <v>27</v>
+      </c>
+      <c r="B30">
+        <f t="shared" si="1"/>
+        <v>-3</v>
+      </c>
+      <c r="C30">
+        <f t="shared" si="2"/>
+        <v>177</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31">
+        <v>28</v>
+      </c>
+      <c r="B31">
+        <f t="shared" si="1"/>
+        <v>-2</v>
+      </c>
+      <c r="C31">
+        <f t="shared" si="2"/>
+        <v>178</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32">
+        <v>29</v>
+      </c>
+      <c r="B32">
+        <f t="shared" si="1"/>
+        <v>-1</v>
+      </c>
+      <c r="C32">
+        <f t="shared" si="2"/>
+        <v>179</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33">
+        <v>30</v>
+      </c>
+      <c r="B33">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="C33">
+        <f t="shared" si="2"/>
+        <v>180</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34">
+        <v>31</v>
+      </c>
+      <c r="B34">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="C34">
+        <f t="shared" si="2"/>
+        <v>179</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35">
+        <v>32</v>
+      </c>
+      <c r="B35">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="C35">
+        <f t="shared" si="2"/>
+        <v>178</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36">
+        <v>33</v>
+      </c>
+      <c r="B36">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="C36">
+        <f t="shared" si="2"/>
+        <v>177</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37">
+        <v>34</v>
+      </c>
+      <c r="B37">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="C37">
+        <f t="shared" si="2"/>
+        <v>176</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38">
+        <v>35</v>
+      </c>
+      <c r="B38">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="C38">
+        <f t="shared" si="2"/>
+        <v>175</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39">
+        <v>36</v>
+      </c>
+      <c r="B39">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="C39">
+        <f t="shared" si="2"/>
+        <v>174</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40">
+        <v>37</v>
+      </c>
+      <c r="B40">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="C40">
+        <f t="shared" si="2"/>
+        <v>173</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41">
+        <v>38</v>
+      </c>
+      <c r="B41">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="C41">
+        <f t="shared" si="2"/>
+        <v>172</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42">
+        <v>39</v>
+      </c>
+      <c r="B42">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="C42">
+        <f t="shared" si="2"/>
+        <v>171</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43">
+        <v>40</v>
+      </c>
+      <c r="B43">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="C43">
+        <f t="shared" si="2"/>
+        <v>170</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44">
+        <v>41</v>
+      </c>
+      <c r="B44">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="C44">
+        <f t="shared" si="2"/>
+        <v>169</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45">
+        <v>42</v>
+      </c>
+      <c r="B45">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="C45">
+        <f t="shared" si="2"/>
+        <v>168</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46">
+        <v>43</v>
+      </c>
+      <c r="B46">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="C46">
+        <f t="shared" si="2"/>
+        <v>167</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47">
+        <v>44</v>
+      </c>
+      <c r="B47">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="C47">
+        <f t="shared" si="2"/>
+        <v>166</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48">
+        <v>45</v>
+      </c>
+      <c r="B48">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="C48">
+        <f t="shared" si="2"/>
+        <v>165</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49">
+        <v>46</v>
+      </c>
+      <c r="B49">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="C49">
+        <f t="shared" si="2"/>
+        <v>164</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50">
+        <v>47</v>
+      </c>
+      <c r="B50">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
+      <c r="C50">
+        <f t="shared" si="2"/>
+        <v>163</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51">
+        <v>48</v>
+      </c>
+      <c r="B51">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="C51">
+        <f t="shared" si="2"/>
+        <v>162</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52">
+        <v>49</v>
+      </c>
+      <c r="B52">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+      <c r="C52">
+        <f t="shared" si="2"/>
+        <v>161</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="A53">
+        <v>50</v>
+      </c>
+      <c r="B53">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="C53">
+        <f t="shared" si="2"/>
+        <v>160</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
+      <c r="A54">
+        <v>51</v>
+      </c>
+      <c r="B54">
+        <f t="shared" si="1"/>
+        <v>21</v>
+      </c>
+      <c r="C54">
+        <f t="shared" si="2"/>
+        <v>159</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="A55">
+        <v>52</v>
+      </c>
+      <c r="B55">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+      <c r="C55">
+        <f t="shared" si="2"/>
+        <v>158</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="A56">
+        <v>53</v>
+      </c>
+      <c r="B56">
+        <f t="shared" si="1"/>
+        <v>23</v>
+      </c>
+      <c r="C56">
+        <f t="shared" si="2"/>
+        <v>157</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
+      <c r="A57">
+        <v>54</v>
+      </c>
+      <c r="B57">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+      <c r="C57">
+        <f t="shared" si="2"/>
+        <v>156</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
+      <c r="A58">
+        <v>55</v>
+      </c>
+      <c r="B58">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="C58">
+        <f t="shared" si="2"/>
+        <v>155</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3">
+      <c r="A59">
+        <v>56</v>
+      </c>
+      <c r="B59">
+        <f t="shared" si="1"/>
+        <v>26</v>
+      </c>
+      <c r="C59">
+        <f t="shared" si="2"/>
+        <v>154</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3">
+      <c r="A60">
+        <v>57</v>
+      </c>
+      <c r="B60">
+        <f t="shared" si="1"/>
+        <v>27</v>
+      </c>
+      <c r="C60">
+        <f t="shared" si="2"/>
+        <v>153</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3">
+      <c r="A61">
+        <v>58</v>
+      </c>
+      <c r="B61">
+        <f t="shared" si="1"/>
+        <v>28</v>
+      </c>
+      <c r="C61">
+        <f t="shared" si="2"/>
+        <v>152</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3">
+      <c r="A62">
+        <v>59</v>
+      </c>
+      <c r="B62">
+        <f t="shared" si="1"/>
+        <v>29</v>
+      </c>
+      <c r="C62">
+        <f t="shared" si="2"/>
+        <v>151</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3">
+      <c r="A63">
+        <v>60</v>
+      </c>
+      <c r="B63">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="C63">
+        <f t="shared" si="2"/>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3">
+      <c r="A64">
+        <v>61</v>
+      </c>
+      <c r="B64">
+        <f t="shared" si="1"/>
+        <v>31</v>
+      </c>
+      <c r="C64">
+        <f t="shared" si="2"/>
+        <v>149</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3">
+      <c r="A65">
+        <v>62</v>
+      </c>
+      <c r="B65">
+        <f t="shared" si="1"/>
+        <v>32</v>
+      </c>
+      <c r="C65">
+        <f t="shared" si="2"/>
+        <v>148</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3">
+      <c r="A66">
+        <v>63</v>
+      </c>
+      <c r="B66">
+        <f t="shared" si="1"/>
+        <v>33</v>
+      </c>
+      <c r="C66">
+        <f t="shared" si="2"/>
+        <v>147</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3">
+      <c r="A67">
+        <v>64</v>
+      </c>
+      <c r="B67">
+        <f t="shared" si="1"/>
+        <v>34</v>
+      </c>
+      <c r="C67">
+        <f t="shared" si="2"/>
+        <v>146</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
+      <c r="A68">
+        <v>65</v>
+      </c>
+      <c r="B68">
+        <f t="shared" ref="B68:B131" si="3">A68-$F$1</f>
+        <v>35</v>
+      </c>
+      <c r="C68">
+        <f t="shared" si="2"/>
+        <v>145</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3">
+      <c r="A69">
+        <v>66</v>
+      </c>
+      <c r="B69">
+        <f t="shared" si="3"/>
+        <v>36</v>
+      </c>
+      <c r="C69">
+        <f t="shared" si="2"/>
+        <v>144</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3">
+      <c r="A70">
+        <v>67</v>
+      </c>
+      <c r="B70">
+        <f t="shared" si="3"/>
+        <v>37</v>
+      </c>
+      <c r="C70">
+        <f t="shared" si="2"/>
+        <v>143</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3">
+      <c r="A71">
+        <v>68</v>
+      </c>
+      <c r="B71">
+        <f t="shared" si="3"/>
+        <v>38</v>
+      </c>
+      <c r="C71">
+        <f t="shared" si="2"/>
+        <v>142</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3">
+      <c r="A72">
+        <v>69</v>
+      </c>
+      <c r="B72">
+        <f t="shared" si="3"/>
+        <v>39</v>
+      </c>
+      <c r="C72">
+        <f t="shared" si="2"/>
+        <v>141</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3">
+      <c r="A73">
+        <v>70</v>
+      </c>
+      <c r="B73">
+        <f t="shared" si="3"/>
+        <v>40</v>
+      </c>
+      <c r="C73">
+        <f t="shared" si="2"/>
+        <v>140</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3">
+      <c r="A74">
+        <v>71</v>
+      </c>
+      <c r="B74">
+        <f t="shared" si="3"/>
+        <v>41</v>
+      </c>
+      <c r="C74">
+        <f t="shared" si="2"/>
+        <v>139</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3">
+      <c r="A75">
+        <v>72</v>
+      </c>
+      <c r="B75">
+        <f t="shared" si="3"/>
+        <v>42</v>
+      </c>
+      <c r="C75">
+        <f t="shared" si="2"/>
+        <v>138</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3">
+      <c r="A76">
+        <v>73</v>
+      </c>
+      <c r="B76">
+        <f t="shared" si="3"/>
+        <v>43</v>
+      </c>
+      <c r="C76">
+        <f t="shared" si="2"/>
+        <v>137</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3">
+      <c r="A77">
+        <v>74</v>
+      </c>
+      <c r="B77">
+        <f t="shared" si="3"/>
+        <v>44</v>
+      </c>
+      <c r="C77">
+        <f t="shared" si="2"/>
+        <v>136</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3">
+      <c r="A78">
+        <v>75</v>
+      </c>
+      <c r="B78">
+        <f t="shared" si="3"/>
+        <v>45</v>
+      </c>
+      <c r="C78">
+        <f t="shared" si="2"/>
+        <v>135</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3">
+      <c r="A79">
+        <v>76</v>
+      </c>
+      <c r="B79">
+        <f t="shared" si="3"/>
+        <v>46</v>
+      </c>
+      <c r="C79">
+        <f t="shared" si="2"/>
+        <v>134</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3">
+      <c r="A80">
+        <v>77</v>
+      </c>
+      <c r="B80">
+        <f t="shared" si="3"/>
+        <v>47</v>
+      </c>
+      <c r="C80">
+        <f t="shared" si="2"/>
+        <v>133</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3">
+      <c r="A81">
+        <v>78</v>
+      </c>
+      <c r="B81">
+        <f t="shared" si="3"/>
+        <v>48</v>
+      </c>
+      <c r="C81">
+        <f t="shared" si="2"/>
+        <v>132</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3">
+      <c r="A82">
+        <v>79</v>
+      </c>
+      <c r="B82">
+        <f t="shared" si="3"/>
+        <v>49</v>
+      </c>
+      <c r="C82">
+        <f t="shared" si="2"/>
+        <v>131</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3">
+      <c r="A83">
+        <v>80</v>
+      </c>
+      <c r="B83">
+        <f t="shared" si="3"/>
+        <v>50</v>
+      </c>
+      <c r="C83">
+        <f t="shared" si="2"/>
+        <v>130</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3">
+      <c r="A84">
+        <v>81</v>
+      </c>
+      <c r="B84">
+        <f t="shared" si="3"/>
+        <v>51</v>
+      </c>
+      <c r="C84">
+        <f t="shared" si="2"/>
+        <v>129</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3">
+      <c r="A85">
+        <v>82</v>
+      </c>
+      <c r="B85">
+        <f t="shared" si="3"/>
+        <v>52</v>
+      </c>
+      <c r="C85">
+        <f t="shared" si="2"/>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3">
+      <c r="A86">
+        <v>83</v>
+      </c>
+      <c r="B86">
+        <f t="shared" si="3"/>
+        <v>53</v>
+      </c>
+      <c r="C86">
+        <f t="shared" si="2"/>
+        <v>127</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3">
+      <c r="A87">
+        <v>84</v>
+      </c>
+      <c r="B87">
+        <f t="shared" si="3"/>
+        <v>54</v>
+      </c>
+      <c r="C87">
+        <f t="shared" ref="C87:C150" si="4">180-ABS(B87)</f>
+        <v>126</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3">
+      <c r="A88">
+        <v>85</v>
+      </c>
+      <c r="B88">
+        <f t="shared" si="3"/>
+        <v>55</v>
+      </c>
+      <c r="C88">
+        <f t="shared" si="4"/>
+        <v>125</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3">
+      <c r="A89">
+        <v>86</v>
+      </c>
+      <c r="B89">
+        <f t="shared" si="3"/>
+        <v>56</v>
+      </c>
+      <c r="C89">
+        <f t="shared" si="4"/>
+        <v>124</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3">
+      <c r="A90">
+        <v>87</v>
+      </c>
+      <c r="B90">
+        <f t="shared" si="3"/>
+        <v>57</v>
+      </c>
+      <c r="C90">
+        <f t="shared" si="4"/>
+        <v>123</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3">
+      <c r="A91">
+        <v>88</v>
+      </c>
+      <c r="B91">
+        <f t="shared" si="3"/>
+        <v>58</v>
+      </c>
+      <c r="C91">
+        <f t="shared" si="4"/>
+        <v>122</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3">
+      <c r="A92">
+        <v>89</v>
+      </c>
+      <c r="B92">
+        <f t="shared" si="3"/>
+        <v>59</v>
+      </c>
+      <c r="C92">
+        <f t="shared" si="4"/>
+        <v>121</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3">
+      <c r="A93">
+        <v>90</v>
+      </c>
+      <c r="B93">
+        <f t="shared" si="3"/>
+        <v>60</v>
+      </c>
+      <c r="C93">
+        <f t="shared" si="4"/>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3">
+      <c r="A94">
+        <v>91</v>
+      </c>
+      <c r="B94">
+        <f t="shared" si="3"/>
+        <v>61</v>
+      </c>
+      <c r="C94">
+        <f t="shared" si="4"/>
+        <v>119</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3">
+      <c r="A95">
+        <v>92</v>
+      </c>
+      <c r="B95">
+        <f t="shared" si="3"/>
+        <v>62</v>
+      </c>
+      <c r="C95">
+        <f t="shared" si="4"/>
+        <v>118</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3">
+      <c r="A96">
+        <v>93</v>
+      </c>
+      <c r="B96">
+        <f t="shared" si="3"/>
+        <v>63</v>
+      </c>
+      <c r="C96">
+        <f t="shared" si="4"/>
+        <v>117</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3">
+      <c r="A97">
+        <v>94</v>
+      </c>
+      <c r="B97">
+        <f t="shared" si="3"/>
+        <v>64</v>
+      </c>
+      <c r="C97">
+        <f t="shared" si="4"/>
+        <v>116</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3">
+      <c r="A98">
+        <v>95</v>
+      </c>
+      <c r="B98">
+        <f t="shared" si="3"/>
+        <v>65</v>
+      </c>
+      <c r="C98">
+        <f t="shared" si="4"/>
+        <v>115</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3">
+      <c r="A99">
+        <v>96</v>
+      </c>
+      <c r="B99">
+        <f t="shared" si="3"/>
+        <v>66</v>
+      </c>
+      <c r="C99">
+        <f t="shared" si="4"/>
+        <v>114</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3">
+      <c r="A100">
+        <v>97</v>
+      </c>
+      <c r="B100">
+        <f t="shared" si="3"/>
+        <v>67</v>
+      </c>
+      <c r="C100">
+        <f t="shared" si="4"/>
+        <v>113</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3">
+      <c r="A101">
+        <v>98</v>
+      </c>
+      <c r="B101">
+        <f t="shared" si="3"/>
+        <v>68</v>
+      </c>
+      <c r="C101">
+        <f t="shared" si="4"/>
+        <v>112</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3">
+      <c r="A102">
+        <v>99</v>
+      </c>
+      <c r="B102">
+        <f t="shared" si="3"/>
+        <v>69</v>
+      </c>
+      <c r="C102">
+        <f t="shared" si="4"/>
+        <v>111</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3">
+      <c r="A103">
+        <v>100</v>
+      </c>
+      <c r="B103">
+        <f t="shared" si="3"/>
+        <v>70</v>
+      </c>
+      <c r="C103">
+        <f t="shared" si="4"/>
+        <v>110</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3">
+      <c r="A104">
+        <v>101</v>
+      </c>
+      <c r="B104">
+        <f t="shared" si="3"/>
+        <v>71</v>
+      </c>
+      <c r="C104">
+        <f t="shared" si="4"/>
+        <v>109</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3">
+      <c r="A105">
+        <v>102</v>
+      </c>
+      <c r="B105">
+        <f t="shared" si="3"/>
+        <v>72</v>
+      </c>
+      <c r="C105">
+        <f t="shared" si="4"/>
+        <v>108</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3">
+      <c r="A106">
+        <v>103</v>
+      </c>
+      <c r="B106">
+        <f t="shared" si="3"/>
+        <v>73</v>
+      </c>
+      <c r="C106">
+        <f t="shared" si="4"/>
+        <v>107</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3">
+      <c r="A107">
+        <v>104</v>
+      </c>
+      <c r="B107">
+        <f t="shared" si="3"/>
+        <v>74</v>
+      </c>
+      <c r="C107">
+        <f t="shared" si="4"/>
+        <v>106</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3">
+      <c r="A108">
+        <v>105</v>
+      </c>
+      <c r="B108">
+        <f t="shared" si="3"/>
+        <v>75</v>
+      </c>
+      <c r="C108">
+        <f t="shared" si="4"/>
+        <v>105</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3">
+      <c r="A109">
+        <v>106</v>
+      </c>
+      <c r="B109">
+        <f t="shared" si="3"/>
+        <v>76</v>
+      </c>
+      <c r="C109">
+        <f t="shared" si="4"/>
+        <v>104</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3">
+      <c r="A110">
+        <v>107</v>
+      </c>
+      <c r="B110">
+        <f t="shared" si="3"/>
+        <v>77</v>
+      </c>
+      <c r="C110">
+        <f t="shared" si="4"/>
+        <v>103</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3">
+      <c r="A111">
+        <v>108</v>
+      </c>
+      <c r="B111">
+        <f t="shared" si="3"/>
+        <v>78</v>
+      </c>
+      <c r="C111">
+        <f t="shared" si="4"/>
+        <v>102</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3">
+      <c r="A112">
+        <v>109</v>
+      </c>
+      <c r="B112">
+        <f t="shared" si="3"/>
+        <v>79</v>
+      </c>
+      <c r="C112">
+        <f t="shared" si="4"/>
+        <v>101</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3">
+      <c r="A113">
+        <v>110</v>
+      </c>
+      <c r="B113">
+        <f t="shared" si="3"/>
+        <v>80</v>
+      </c>
+      <c r="C113">
+        <f t="shared" si="4"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3">
+      <c r="A114">
+        <v>111</v>
+      </c>
+      <c r="B114">
+        <f t="shared" si="3"/>
+        <v>81</v>
+      </c>
+      <c r="C114">
+        <f t="shared" si="4"/>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3">
+      <c r="A115">
+        <v>112</v>
+      </c>
+      <c r="B115">
+        <f t="shared" si="3"/>
+        <v>82</v>
+      </c>
+      <c r="C115">
+        <f t="shared" si="4"/>
+        <v>98</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3">
+      <c r="A116">
+        <v>113</v>
+      </c>
+      <c r="B116">
+        <f t="shared" si="3"/>
+        <v>83</v>
+      </c>
+      <c r="C116">
+        <f t="shared" si="4"/>
+        <v>97</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3">
+      <c r="A117">
+        <v>114</v>
+      </c>
+      <c r="B117">
+        <f t="shared" si="3"/>
+        <v>84</v>
+      </c>
+      <c r="C117">
+        <f t="shared" si="4"/>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3">
+      <c r="A118">
+        <v>115</v>
+      </c>
+      <c r="B118">
+        <f t="shared" si="3"/>
+        <v>85</v>
+      </c>
+      <c r="C118">
+        <f t="shared" si="4"/>
+        <v>95</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3">
+      <c r="A119">
+        <v>116</v>
+      </c>
+      <c r="B119">
+        <f t="shared" si="3"/>
+        <v>86</v>
+      </c>
+      <c r="C119">
+        <f t="shared" si="4"/>
+        <v>94</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3">
+      <c r="A120">
+        <v>117</v>
+      </c>
+      <c r="B120">
+        <f t="shared" si="3"/>
+        <v>87</v>
+      </c>
+      <c r="C120">
+        <f t="shared" si="4"/>
+        <v>93</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3">
+      <c r="A121">
+        <v>118</v>
+      </c>
+      <c r="B121">
+        <f t="shared" si="3"/>
+        <v>88</v>
+      </c>
+      <c r="C121">
+        <f t="shared" si="4"/>
+        <v>92</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3">
+      <c r="A122">
+        <v>119</v>
+      </c>
+      <c r="B122">
+        <f t="shared" si="3"/>
+        <v>89</v>
+      </c>
+      <c r="C122">
+        <f t="shared" si="4"/>
+        <v>91</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3">
+      <c r="A123">
+        <v>120</v>
+      </c>
+      <c r="B123">
+        <f t="shared" si="3"/>
+        <v>90</v>
+      </c>
+      <c r="C123">
+        <f t="shared" si="4"/>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3">
+      <c r="A124">
+        <v>121</v>
+      </c>
+      <c r="B124">
+        <f t="shared" si="3"/>
+        <v>91</v>
+      </c>
+      <c r="C124">
+        <f t="shared" si="4"/>
+        <v>89</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3">
+      <c r="A125">
+        <v>122</v>
+      </c>
+      <c r="B125">
+        <f t="shared" si="3"/>
+        <v>92</v>
+      </c>
+      <c r="C125">
+        <f t="shared" si="4"/>
+        <v>88</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3">
+      <c r="A126">
+        <v>123</v>
+      </c>
+      <c r="B126">
+        <f t="shared" si="3"/>
+        <v>93</v>
+      </c>
+      <c r="C126">
+        <f t="shared" si="4"/>
+        <v>87</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3">
+      <c r="A127">
+        <v>124</v>
+      </c>
+      <c r="B127">
+        <f t="shared" si="3"/>
+        <v>94</v>
+      </c>
+      <c r="C127">
+        <f t="shared" si="4"/>
+        <v>86</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3">
+      <c r="A128">
+        <v>125</v>
+      </c>
+      <c r="B128">
+        <f t="shared" si="3"/>
+        <v>95</v>
+      </c>
+      <c r="C128">
+        <f t="shared" si="4"/>
+        <v>85</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3">
+      <c r="A129">
+        <v>126</v>
+      </c>
+      <c r="B129">
+        <f t="shared" si="3"/>
+        <v>96</v>
+      </c>
+      <c r="C129">
+        <f t="shared" si="4"/>
+        <v>84</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3">
+      <c r="A130">
+        <v>127</v>
+      </c>
+      <c r="B130">
+        <f t="shared" si="3"/>
+        <v>97</v>
+      </c>
+      <c r="C130">
+        <f t="shared" si="4"/>
+        <v>83</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3">
+      <c r="A131">
+        <v>128</v>
+      </c>
+      <c r="B131">
+        <f t="shared" si="3"/>
+        <v>98</v>
+      </c>
+      <c r="C131">
+        <f t="shared" si="4"/>
+        <v>82</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3">
+      <c r="A132">
+        <v>129</v>
+      </c>
+      <c r="B132">
+        <f t="shared" ref="B132:B182" si="5">A132-$F$1</f>
+        <v>99</v>
+      </c>
+      <c r="C132">
+        <f t="shared" si="4"/>
+        <v>81</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3">
+      <c r="A133">
+        <v>130</v>
+      </c>
+      <c r="B133">
+        <f t="shared" si="5"/>
+        <v>100</v>
+      </c>
+      <c r="C133">
+        <f t="shared" si="4"/>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3">
+      <c r="A134">
+        <v>131</v>
+      </c>
+      <c r="B134">
+        <f t="shared" si="5"/>
+        <v>101</v>
+      </c>
+      <c r="C134">
+        <f t="shared" si="4"/>
+        <v>79</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3">
+      <c r="A135">
+        <v>132</v>
+      </c>
+      <c r="B135">
+        <f t="shared" si="5"/>
+        <v>102</v>
+      </c>
+      <c r="C135">
+        <f t="shared" si="4"/>
+        <v>78</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3">
+      <c r="A136">
+        <v>133</v>
+      </c>
+      <c r="B136">
+        <f t="shared" si="5"/>
+        <v>103</v>
+      </c>
+      <c r="C136">
+        <f t="shared" si="4"/>
+        <v>77</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3">
+      <c r="A137">
+        <v>134</v>
+      </c>
+      <c r="B137">
+        <f t="shared" si="5"/>
+        <v>104</v>
+      </c>
+      <c r="C137">
+        <f t="shared" si="4"/>
+        <v>76</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3">
+      <c r="A138">
+        <v>135</v>
+      </c>
+      <c r="B138">
+        <f t="shared" si="5"/>
+        <v>105</v>
+      </c>
+      <c r="C138">
+        <f t="shared" si="4"/>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3">
+      <c r="A139">
+        <v>136</v>
+      </c>
+      <c r="B139">
+        <f t="shared" si="5"/>
+        <v>106</v>
+      </c>
+      <c r="C139">
+        <f t="shared" si="4"/>
+        <v>74</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3">
+      <c r="A140">
+        <v>137</v>
+      </c>
+      <c r="B140">
+        <f t="shared" si="5"/>
+        <v>107</v>
+      </c>
+      <c r="C140">
+        <f t="shared" si="4"/>
+        <v>73</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3">
+      <c r="A141">
+        <v>138</v>
+      </c>
+      <c r="B141">
+        <f t="shared" si="5"/>
+        <v>108</v>
+      </c>
+      <c r="C141">
+        <f t="shared" si="4"/>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3">
+      <c r="A142">
+        <v>139</v>
+      </c>
+      <c r="B142">
+        <f t="shared" si="5"/>
+        <v>109</v>
+      </c>
+      <c r="C142">
+        <f t="shared" si="4"/>
+        <v>71</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3">
+      <c r="A143">
+        <v>140</v>
+      </c>
+      <c r="B143">
+        <f t="shared" si="5"/>
+        <v>110</v>
+      </c>
+      <c r="C143">
+        <f t="shared" si="4"/>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3">
+      <c r="A144">
+        <v>141</v>
+      </c>
+      <c r="B144">
+        <f t="shared" si="5"/>
+        <v>111</v>
+      </c>
+      <c r="C144">
+        <f t="shared" si="4"/>
+        <v>69</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3">
+      <c r="A145">
+        <v>142</v>
+      </c>
+      <c r="B145">
+        <f t="shared" si="5"/>
+        <v>112</v>
+      </c>
+      <c r="C145">
+        <f t="shared" si="4"/>
+        <v>68</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3">
+      <c r="A146">
+        <v>143</v>
+      </c>
+      <c r="B146">
+        <f t="shared" si="5"/>
+        <v>113</v>
+      </c>
+      <c r="C146">
+        <f t="shared" si="4"/>
+        <v>67</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3">
+      <c r="A147">
+        <v>144</v>
+      </c>
+      <c r="B147">
+        <f t="shared" si="5"/>
+        <v>114</v>
+      </c>
+      <c r="C147">
+        <f t="shared" si="4"/>
+        <v>66</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3">
+      <c r="A148">
+        <v>145</v>
+      </c>
+      <c r="B148">
+        <f t="shared" si="5"/>
+        <v>115</v>
+      </c>
+      <c r="C148">
+        <f t="shared" si="4"/>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3">
+      <c r="A149">
+        <v>146</v>
+      </c>
+      <c r="B149">
+        <f t="shared" si="5"/>
+        <v>116</v>
+      </c>
+      <c r="C149">
+        <f t="shared" si="4"/>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3">
+      <c r="A150">
+        <v>147</v>
+      </c>
+      <c r="B150">
+        <f t="shared" si="5"/>
+        <v>117</v>
+      </c>
+      <c r="C150">
+        <f t="shared" si="4"/>
+        <v>63</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3">
+      <c r="A151">
+        <v>148</v>
+      </c>
+      <c r="B151">
+        <f t="shared" si="5"/>
+        <v>118</v>
+      </c>
+      <c r="C151">
+        <f t="shared" ref="C151:C182" si="6">180-ABS(B151)</f>
+        <v>62</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3">
+      <c r="A152">
+        <v>149</v>
+      </c>
+      <c r="B152">
+        <f t="shared" si="5"/>
+        <v>119</v>
+      </c>
+      <c r="C152">
+        <f t="shared" si="6"/>
+        <v>61</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3">
+      <c r="A153">
+        <v>150</v>
+      </c>
+      <c r="B153">
+        <f t="shared" si="5"/>
+        <v>120</v>
+      </c>
+      <c r="C153">
+        <f t="shared" si="6"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3">
+      <c r="A154">
+        <v>151</v>
+      </c>
+      <c r="B154">
+        <f t="shared" si="5"/>
+        <v>121</v>
+      </c>
+      <c r="C154">
+        <f t="shared" si="6"/>
+        <v>59</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3">
+      <c r="A155">
+        <v>152</v>
+      </c>
+      <c r="B155">
+        <f t="shared" si="5"/>
+        <v>122</v>
+      </c>
+      <c r="C155">
+        <f t="shared" si="6"/>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3">
+      <c r="A156">
+        <v>153</v>
+      </c>
+      <c r="B156">
+        <f t="shared" si="5"/>
+        <v>123</v>
+      </c>
+      <c r="C156">
+        <f t="shared" si="6"/>
+        <v>57</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3">
+      <c r="A157">
+        <v>154</v>
+      </c>
+      <c r="B157">
+        <f t="shared" si="5"/>
+        <v>124</v>
+      </c>
+      <c r="C157">
+        <f t="shared" si="6"/>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3">
+      <c r="A158">
+        <v>155</v>
+      </c>
+      <c r="B158">
+        <f t="shared" si="5"/>
+        <v>125</v>
+      </c>
+      <c r="C158">
+        <f t="shared" si="6"/>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3">
+      <c r="A159">
+        <v>156</v>
+      </c>
+      <c r="B159">
+        <f t="shared" si="5"/>
+        <v>126</v>
+      </c>
+      <c r="C159">
+        <f t="shared" si="6"/>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3">
+      <c r="A160">
+        <v>157</v>
+      </c>
+      <c r="B160">
+        <f t="shared" si="5"/>
+        <v>127</v>
+      </c>
+      <c r="C160">
+        <f t="shared" si="6"/>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3">
+      <c r="A161">
+        <v>158</v>
+      </c>
+      <c r="B161">
+        <f t="shared" si="5"/>
+        <v>128</v>
+      </c>
+      <c r="C161">
+        <f t="shared" si="6"/>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3">
+      <c r="A162">
+        <v>159</v>
+      </c>
+      <c r="B162">
+        <f t="shared" si="5"/>
+        <v>129</v>
+      </c>
+      <c r="C162">
+        <f t="shared" si="6"/>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3">
+      <c r="A163">
+        <v>160</v>
+      </c>
+      <c r="B163">
+        <f t="shared" si="5"/>
+        <v>130</v>
+      </c>
+      <c r="C163">
+        <f t="shared" si="6"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3">
+      <c r="A164">
+        <v>161</v>
+      </c>
+      <c r="B164">
+        <f t="shared" si="5"/>
+        <v>131</v>
+      </c>
+      <c r="C164">
+        <f t="shared" si="6"/>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3">
+      <c r="A165">
+        <v>162</v>
+      </c>
+      <c r="B165">
+        <f t="shared" si="5"/>
+        <v>132</v>
+      </c>
+      <c r="C165">
+        <f t="shared" si="6"/>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3">
+      <c r="A166">
+        <v>163</v>
+      </c>
+      <c r="B166">
+        <f t="shared" si="5"/>
+        <v>133</v>
+      </c>
+      <c r="C166">
+        <f t="shared" si="6"/>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3">
+      <c r="A167">
+        <v>164</v>
+      </c>
+      <c r="B167">
+        <f t="shared" si="5"/>
+        <v>134</v>
+      </c>
+      <c r="C167">
+        <f t="shared" si="6"/>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3">
+      <c r="A168">
+        <v>165</v>
+      </c>
+      <c r="B168">
+        <f t="shared" si="5"/>
+        <v>135</v>
+      </c>
+      <c r="C168">
+        <f t="shared" si="6"/>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3">
+      <c r="A169">
+        <v>166</v>
+      </c>
+      <c r="B169">
+        <f t="shared" si="5"/>
+        <v>136</v>
+      </c>
+      <c r="C169">
+        <f t="shared" si="6"/>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3">
+      <c r="A170">
+        <v>167</v>
+      </c>
+      <c r="B170">
+        <f t="shared" si="5"/>
+        <v>137</v>
+      </c>
+      <c r="C170">
+        <f t="shared" si="6"/>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3">
+      <c r="A171">
+        <v>168</v>
+      </c>
+      <c r="B171">
+        <f t="shared" si="5"/>
+        <v>138</v>
+      </c>
+      <c r="C171">
+        <f t="shared" si="6"/>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3">
+      <c r="A172">
+        <v>169</v>
+      </c>
+      <c r="B172">
+        <f t="shared" si="5"/>
+        <v>139</v>
+      </c>
+      <c r="C172">
+        <f t="shared" si="6"/>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3">
+      <c r="A173">
+        <v>170</v>
+      </c>
+      <c r="B173">
+        <f t="shared" si="5"/>
+        <v>140</v>
+      </c>
+      <c r="C173">
+        <f t="shared" si="6"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3">
+      <c r="A174">
+        <v>171</v>
+      </c>
+      <c r="B174">
+        <f t="shared" si="5"/>
+        <v>141</v>
+      </c>
+      <c r="C174">
+        <f t="shared" si="6"/>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3">
+      <c r="A175">
+        <v>172</v>
+      </c>
+      <c r="B175">
+        <f t="shared" si="5"/>
+        <v>142</v>
+      </c>
+      <c r="C175">
+        <f t="shared" si="6"/>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3">
+      <c r="A176">
+        <v>173</v>
+      </c>
+      <c r="B176">
+        <f t="shared" si="5"/>
+        <v>143</v>
+      </c>
+      <c r="C176">
+        <f t="shared" si="6"/>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3">
+      <c r="A177">
+        <v>174</v>
+      </c>
+      <c r="B177">
+        <f t="shared" si="5"/>
+        <v>144</v>
+      </c>
+      <c r="C177">
+        <f t="shared" si="6"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3">
+      <c r="A178">
+        <v>175</v>
+      </c>
+      <c r="B178">
+        <f t="shared" si="5"/>
+        <v>145</v>
+      </c>
+      <c r="C178">
+        <f t="shared" si="6"/>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3">
+      <c r="A179">
+        <v>176</v>
+      </c>
+      <c r="B179">
+        <f t="shared" si="5"/>
+        <v>146</v>
+      </c>
+      <c r="C179">
+        <f t="shared" si="6"/>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3">
+      <c r="A180">
+        <v>177</v>
+      </c>
+      <c r="B180">
+        <f t="shared" si="5"/>
+        <v>147</v>
+      </c>
+      <c r="C180">
+        <f t="shared" si="6"/>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3">
+      <c r="A181">
+        <v>178</v>
+      </c>
+      <c r="B181">
+        <f t="shared" si="5"/>
+        <v>148</v>
+      </c>
+      <c r="C181">
+        <f t="shared" si="6"/>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3">
+      <c r="A182">
+        <v>179</v>
+      </c>
+      <c r="B182">
+        <f t="shared" si="5"/>
+        <v>149</v>
+      </c>
+      <c r="C182">
+        <f t="shared" si="6"/>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>